<commit_message>
version 10 after demo
</commit_message>
<xml_diff>
--- a/Mu Calculationxlsx.xlsx
+++ b/Mu Calculationxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K E S SRINIVAS\Documents\ABS Project SAE\ABS-Simulink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849E73F2-9AE2-4F8B-BB7F-1BABAF64993E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A82EA46-E60E-4DD8-9915-9A31780DB090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B4BA73F7-7503-47F0-9BBA-406C6E08481F}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Lambda</t>
-  </si>
-  <si>
     <t>Mu</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>C4</t>
+  </si>
+  <si>
+    <t>Slip Ratio</t>
   </si>
 </sst>
 </file>
@@ -2428,304 +2428,304 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.7709245999152996E-2</c:v>
+                  <c:v>0.13367579168737431</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1087640264485505</c:v>
+                  <c:v>0.25193739912716762</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15391682540643978</c:v>
+                  <c:v>0.35652785154245797</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19383503636238386</c:v>
+                  <c:v>0.44899307717298803</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.22911058424160835</c:v>
+                  <c:v>0.53070419136828384</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26026845935729798</c:v>
+                  <c:v>0.60287726435293676</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.28777428634729518</c:v>
+                  <c:v>0.6665908536616203</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.31204103721874094</c:v>
+                  <c:v>0.72280155401401092</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33343498528456106</c:v>
+                  <c:v>0.77235778881664641</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.35228098583141337</c:v>
+                  <c:v>0.81601204212777345</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.36886715965201022</c:v>
+                  <c:v>0.85443170743695518</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.38344904696565174</c:v>
+                  <c:v>0.88820870966941745</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.39625329161523798</c:v>
+                  <c:v>0.91786803913834492</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.40748090865689324</c:v>
+                  <c:v>0.94387532048157996</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.41731018245198204</c:v>
+                  <c:v>0.96664352570626333</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.42589923704414567</c:v>
+                  <c:v>0.98653892812532118</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.43338831587922588</c:v>
+                  <c:v>1.0038863830254112</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.43990180373545545</c:v>
+                  <c:v>1.018974011199246</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.44555002001466543</c:v>
+                  <c:v>1.0320573528661254</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.45043080924890622</c:v>
+                  <c:v>1.0433630518689494</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.45463095175327434</c:v>
+                  <c:v>1.0530921232638424</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.45822741476273376</c:v>
+                  <c:v>1.0614228514121689</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.46128846209093161</c:v>
+                  <c:v>1.0685133603575705</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.46387463830927966</c:v>
+                  <c:v>1.0745038935458884</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.46603964163549538</c:v>
+                  <c:v>1.0795188357553558</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.4678310981162877</c:v>
+                  <c:v>1.0836685063878035</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.4692912482658026</c:v>
+                  <c:v>1.0870507499752817</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.47045755605929412</c:v>
+                  <c:v>1.089752346832888</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.47136324906205507</c:v>
+                  <c:v>1.0918502641955852</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.47203779748080643</c:v>
+                  <c:v>1.0934127658770207</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.47250733904416325</c:v>
+                  <c:v>1.0945003964486066</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.4727950558378034</c:v>
+                  <c:v>1.0951668541280599</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.4729215085272806</c:v>
+                  <c:v>1.0954597649620901</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.47290493278706669</c:v>
+                  <c:v>1.0954213694648429</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.47276150220952812</c:v>
+                  <c:v>1.0950891316115721</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.4725055614842702</c:v>
+                  <c:v>1.094496278967571</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.47214983320966153</c:v>
+                  <c:v>1.0936722817395601</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.47170560131820377</c:v>
+                  <c:v>1.0926432776561545</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.47118287376023948</c:v>
+                  <c:v>1.0914324488030325</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.47059052679145652</c:v>
+                  <c:v>1.0900603558457473</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.4699364329444265</c:v>
+                  <c:v>1.0885452344587714</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.46922757452917563</c:v>
+                  <c:v>1.0869032582344709</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.46847014429916151</c:v>
+                  <c:v>1.0851487718624504</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.4676696347339856</c:v>
+                  <c:v>1.0832944979410795</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.46683091722605441</c:v>
+                  <c:v>1.0813517204028595</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.46595831231284873</c:v>
+                  <c:v>1.0793304471981331</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.46505565196735787</c:v>
+                  <c:v>1.0772395545825881</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.46412633484473864</c:v>
+                  <c:v>1.0750869150887958</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.46317337528170743</c:v>
+                  <c:v>1.0728795110267826</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.46219944675510105</c:v>
+                  <c:v>1.0706235351500064</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.46120692042616274</c:v>
+                  <c:v>1.068324479938068</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.46019789932625865</c:v>
+                  <c:v>1.0659872167833748</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.45917424867688567</c:v>
+                  <c:v>1.0636160662234067</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.45813762278110909</c:v>
+                  <c:v>1.0612148602311537</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.45708948887412537</c:v>
+                  <c:v>1.0587869974617721</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.4560311482768164</c:v>
+                  <c:v>1.0563354922519788</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.45496375515726656</c:v>
+                  <c:v>1.0538630180786102</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.4538883331707374</c:v>
+                  <c:v>1.0513719461029098</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.45280579021800071</c:v>
+                  <c:v>1.0488643793562435</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.45171693153480535</c:v>
+                  <c:v>1.0463421830601083</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.45062247130119337</c:v>
+                  <c:v>1.0438070115175695</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.44952304293803963</c:v>
+                  <c:v>1.0412603319638236</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.44841920823926296</c:v>
+                  <c:v>1.0387034457197521</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.44731146547137141</c:v>
+                  <c:v>1.0361375069534402</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.44620025655711376</c:v>
+                  <c:v>1.033563539320149</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.44508597344680723</c:v>
+                  <c:v>1.03098245072065</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.44396896376919859</c:v>
+                  <c:v>1.0283950463906926</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.44284953584332748</c:v>
+                  <c:v>1.0258020405103181</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.44172796312365159</c:v>
+                  <c:v>1.0232040665004023</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.44060448814251746</c:v>
+                  <c:v>1.0206016861548635</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.43947932600682005</c:v>
+                  <c:v>1.0179953977402094</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.43835266749926072</c:v>
+                  <c:v>1.0153856431791897</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.43722468182891611</c:v>
+                  <c:v>1.0127728144221211</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.43609551907077426</c:v>
+                  <c:v>1.0101572590977501</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.43496531232940927</c:v>
+                  <c:v>1.0075392855251168</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.43383417965798798</c:v>
+                  <c:v>1.0049191671586786</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.432702225760277</c:v>
+                  <c:v>1.0022971465307822</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.43156954350018645</c:v>
+                  <c:v>0.99967343874832271</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.43043621524061609</c:v>
+                  <c:v>0.99704823459400105</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.42930231403090502</c:v>
+                  <c:v>0.99442170327689428</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.42816790466000493</c:v>
+                  <c:v>0.99179399487199016</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.42703304459056107</c:v>
+                  <c:v>0.98916524248386295</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.42589778478736806</c:v>
+                  <c:v>0.98653556416567967</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.42476217045214348</c:v>
+                  <c:v>0.98390506462120619</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.42362624167521495</c:v>
+                  <c:v>0.98127383671435364</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.42249003401351271</c:v>
+                  <c:v>0.97864196280802096</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.42135357900320541</c:v>
+                  <c:v>0.97600951595154772</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.42021690461436517</c:v>
+                  <c:v>0.97337656093388536</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.4190800356542207</c:v>
+                  <c:v>0.97074315521767929</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.41794299412481017</c:v>
+                  <c:v>0.96810934976772411</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.4168057995401907</c:v>
+                  <c:v>0.9654751897857371</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.41566846920777861</c:v>
+                  <c:v>0.96284071536204641</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.41453101847787499</c:v>
+                  <c:v>0.960205962053582</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.41339346096497559</c:v>
+                  <c:v>0.95757096139651265</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.41225580874405476</c:v>
+                  <c:v>0.95493574136090997</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.41111807252465449</c:v>
+                  <c:v>0.95230032675400345</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.40998026180528591</c:v>
+                  <c:v>0.94966473957783049</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.40884238501037318</c:v>
+                  <c:v>0.94702899934644913</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.40770444961170965</c:v>
+                  <c:v>0.94439312336727477</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.40656646223618209</c:v>
+                  <c:v>0.94175712699060887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8372,17 +8372,17 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -8393,7 +8393,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -8407,7 +8407,7 @@
         <v>20</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>40</v>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1.28</v>
@@ -8472,7 +8472,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -8494,7 +8494,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>5.7709245999152996E-2</v>
+        <v>0.13367579168737431</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
@@ -8527,7 +8527,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0.28000000000000003</v>
@@ -8549,7 +8549,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0.1087640264485505</v>
+        <v>0.25193739912716762</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
@@ -8582,7 +8582,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0.03</v>
@@ -8604,7 +8604,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0.15391682540643978</v>
+        <v>0.35652785154245797</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
@@ -8653,7 +8653,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0.19383503636238386</v>
+        <v>0.44899307717298803</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
@@ -8702,7 +8702,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0.22911058424160835</v>
+        <v>0.53070419136828384</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
@@ -8751,7 +8751,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0.26026845935729798</v>
+        <v>0.60287726435293676</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
@@ -8800,7 +8800,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0.28777428634729518</v>
+        <v>0.6665908536616203</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
@@ -8849,7 +8849,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>0.31204103721874094</v>
+        <v>0.72280155401401092</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
@@ -8898,7 +8898,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>0.33343498528456106</v>
+        <v>0.77235778881664641</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
@@ -8947,7 +8947,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>0.35228098583141337</v>
+        <v>0.81601204212777345</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
@@ -8996,7 +8996,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>0.36886715965201022</v>
+        <v>0.85443170743695518</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
@@ -9045,7 +9045,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0.38344904696565174</v>
+        <v>0.88820870966941745</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
@@ -9094,7 +9094,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>0.39625329161523798</v>
+        <v>0.91786803913834492</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
@@ -9143,7 +9143,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0.40748090865689324</v>
+        <v>0.94387532048157996</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
@@ -9192,7 +9192,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0.41731018245198204</v>
+        <v>0.96664352570626333</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
@@ -9241,7 +9241,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>0.42589923704414567</v>
+        <v>0.98653892812532118</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
@@ -9290,7 +9290,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>0.43338831587922588</v>
+        <v>1.0038863830254112</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
@@ -9339,7 +9339,7 @@
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>0.43990180373545545</v>
+        <v>1.018974011199246</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
@@ -9388,7 +9388,7 @@
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>0.44555002001466543</v>
+        <v>1.0320573528661254</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
@@ -9437,7 +9437,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="3"/>
-        <v>0.45043080924890622</v>
+        <v>1.0433630518689494</v>
       </c>
       <c r="H23">
         <f t="shared" si="3"/>
@@ -9486,7 +9486,7 @@
       </c>
       <c r="G24">
         <f t="shared" si="3"/>
-        <v>0.45463095175327434</v>
+        <v>1.0530921232638424</v>
       </c>
       <c r="H24">
         <f t="shared" si="3"/>
@@ -9535,7 +9535,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="3"/>
-        <v>0.45822741476273376</v>
+        <v>1.0614228514121689</v>
       </c>
       <c r="H25">
         <f t="shared" si="3"/>
@@ -9584,7 +9584,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>0.46128846209093161</v>
+        <v>1.0685133603575705</v>
       </c>
       <c r="H26">
         <f t="shared" si="3"/>
@@ -9633,7 +9633,7 @@
       </c>
       <c r="G27">
         <f t="shared" si="4"/>
-        <v>0.46387463830927966</v>
+        <v>1.0745038935458884</v>
       </c>
       <c r="H27">
         <f t="shared" si="4"/>
@@ -9682,7 +9682,7 @@
       </c>
       <c r="G28">
         <f t="shared" si="4"/>
-        <v>0.46603964163549538</v>
+        <v>1.0795188357553558</v>
       </c>
       <c r="H28">
         <f t="shared" si="4"/>
@@ -9731,7 +9731,7 @@
       </c>
       <c r="G29">
         <f t="shared" si="4"/>
-        <v>0.4678310981162877</v>
+        <v>1.0836685063878035</v>
       </c>
       <c r="H29">
         <f t="shared" si="4"/>
@@ -9780,7 +9780,7 @@
       </c>
       <c r="G30">
         <f t="shared" si="4"/>
-        <v>0.4692912482658026</v>
+        <v>1.0870507499752817</v>
       </c>
       <c r="H30">
         <f t="shared" si="4"/>
@@ -9829,7 +9829,7 @@
       </c>
       <c r="G31">
         <f t="shared" si="5"/>
-        <v>0.47045755605929412</v>
+        <v>1.089752346832888</v>
       </c>
       <c r="H31">
         <f t="shared" si="5"/>
@@ -9878,7 +9878,7 @@
       </c>
       <c r="G32">
         <f t="shared" si="5"/>
-        <v>0.47136324906205507</v>
+        <v>1.0918502641955852</v>
       </c>
       <c r="H32">
         <f t="shared" si="5"/>
@@ -9927,7 +9927,7 @@
       </c>
       <c r="G33">
         <f t="shared" si="5"/>
-        <v>0.47203779748080643</v>
+        <v>1.0934127658770207</v>
       </c>
       <c r="H33">
         <f t="shared" si="5"/>
@@ -9976,7 +9976,7 @@
       </c>
       <c r="G34">
         <f t="shared" si="5"/>
-        <v>0.47250733904416325</v>
+        <v>1.0945003964486066</v>
       </c>
       <c r="H34">
         <f t="shared" si="5"/>
@@ -10025,7 +10025,7 @@
       </c>
       <c r="G35">
         <f t="shared" si="6"/>
-        <v>0.4727950558378034</v>
+        <v>1.0951668541280599</v>
       </c>
       <c r="H35">
         <f t="shared" si="6"/>
@@ -10074,7 +10074,7 @@
       </c>
       <c r="G36">
         <f t="shared" si="6"/>
-        <v>0.4729215085272806</v>
+        <v>1.0954597649620901</v>
       </c>
       <c r="H36">
         <f t="shared" si="6"/>
@@ -10123,7 +10123,7 @@
       </c>
       <c r="G37">
         <f t="shared" si="6"/>
-        <v>0.47290493278706669</v>
+        <v>1.0954213694648429</v>
       </c>
       <c r="H37">
         <f t="shared" si="6"/>
@@ -10172,7 +10172,7 @@
       </c>
       <c r="G38">
         <f t="shared" si="6"/>
-        <v>0.47276150220952812</v>
+        <v>1.0950891316115721</v>
       </c>
       <c r="H38">
         <f t="shared" si="6"/>
@@ -10221,7 +10221,7 @@
       </c>
       <c r="G39">
         <f t="shared" si="7"/>
-        <v>0.4725055614842702</v>
+        <v>1.094496278967571</v>
       </c>
       <c r="H39">
         <f t="shared" si="7"/>
@@ -10270,7 +10270,7 @@
       </c>
       <c r="G40">
         <f t="shared" si="7"/>
-        <v>0.47214983320966153</v>
+        <v>1.0936722817395601</v>
       </c>
       <c r="H40">
         <f t="shared" si="7"/>
@@ -10319,7 +10319,7 @@
       </c>
       <c r="G41">
         <f t="shared" si="7"/>
-        <v>0.47170560131820377</v>
+        <v>1.0926432776561545</v>
       </c>
       <c r="H41">
         <f t="shared" si="7"/>
@@ -10368,7 +10368,7 @@
       </c>
       <c r="G42">
         <f t="shared" si="7"/>
-        <v>0.47118287376023948</v>
+        <v>1.0914324488030325</v>
       </c>
       <c r="H42">
         <f t="shared" si="7"/>
@@ -10417,7 +10417,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="8"/>
-        <v>0.47059052679145652</v>
+        <v>1.0900603558457473</v>
       </c>
       <c r="H43">
         <f t="shared" si="8"/>
@@ -10466,7 +10466,7 @@
       </c>
       <c r="G44">
         <f t="shared" si="8"/>
-        <v>0.4699364329444265</v>
+        <v>1.0885452344587714</v>
       </c>
       <c r="H44">
         <f t="shared" si="8"/>
@@ -10515,7 +10515,7 @@
       </c>
       <c r="G45">
         <f t="shared" si="8"/>
-        <v>0.46922757452917563</v>
+        <v>1.0869032582344709</v>
       </c>
       <c r="H45">
         <f t="shared" si="8"/>
@@ -10564,7 +10564,7 @@
       </c>
       <c r="G46">
         <f t="shared" si="8"/>
-        <v>0.46847014429916151</v>
+        <v>1.0851487718624504</v>
       </c>
       <c r="H46">
         <f t="shared" si="8"/>
@@ -10613,7 +10613,7 @@
       </c>
       <c r="G47">
         <f t="shared" si="9"/>
-        <v>0.4676696347339856</v>
+        <v>1.0832944979410795</v>
       </c>
       <c r="H47">
         <f t="shared" si="9"/>
@@ -10662,7 +10662,7 @@
       </c>
       <c r="G48">
         <f t="shared" si="9"/>
-        <v>0.46683091722605441</v>
+        <v>1.0813517204028595</v>
       </c>
       <c r="H48">
         <f t="shared" si="9"/>
@@ -10711,7 +10711,7 @@
       </c>
       <c r="G49">
         <f t="shared" si="9"/>
-        <v>0.46595831231284873</v>
+        <v>1.0793304471981331</v>
       </c>
       <c r="H49">
         <f t="shared" si="9"/>
@@ -10760,7 +10760,7 @@
       </c>
       <c r="G50">
         <f t="shared" si="9"/>
-        <v>0.46505565196735787</v>
+        <v>1.0772395545825881</v>
       </c>
       <c r="H50">
         <f t="shared" si="9"/>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="G51">
         <f t="shared" si="10"/>
-        <v>0.46412633484473864</v>
+        <v>1.0750869150887958</v>
       </c>
       <c r="H51">
         <f t="shared" si="10"/>
@@ -10858,7 +10858,7 @@
       </c>
       <c r="G52">
         <f t="shared" si="10"/>
-        <v>0.46317337528170743</v>
+        <v>1.0728795110267826</v>
       </c>
       <c r="H52">
         <f t="shared" si="10"/>
@@ -10907,7 +10907,7 @@
       </c>
       <c r="G53">
         <f t="shared" si="10"/>
-        <v>0.46219944675510105</v>
+        <v>1.0706235351500064</v>
       </c>
       <c r="H53">
         <f t="shared" si="10"/>
@@ -10956,7 +10956,7 @@
       </c>
       <c r="G54">
         <f t="shared" si="10"/>
-        <v>0.46120692042616274</v>
+        <v>1.068324479938068</v>
       </c>
       <c r="H54">
         <f t="shared" si="10"/>
@@ -11005,7 +11005,7 @@
       </c>
       <c r="G55">
         <f t="shared" si="11"/>
-        <v>0.46019789932625865</v>
+        <v>1.0659872167833748</v>
       </c>
       <c r="H55">
         <f t="shared" si="11"/>
@@ -11054,7 +11054,7 @@
       </c>
       <c r="G56">
         <f t="shared" si="11"/>
-        <v>0.45917424867688567</v>
+        <v>1.0636160662234067</v>
       </c>
       <c r="H56">
         <f t="shared" si="11"/>
@@ -11103,7 +11103,7 @@
       </c>
       <c r="G57">
         <f t="shared" si="11"/>
-        <v>0.45813762278110909</v>
+        <v>1.0612148602311537</v>
       </c>
       <c r="H57">
         <f t="shared" si="11"/>
@@ -11152,7 +11152,7 @@
       </c>
       <c r="G58">
         <f t="shared" si="11"/>
-        <v>0.45708948887412537</v>
+        <v>1.0587869974617721</v>
       </c>
       <c r="H58">
         <f t="shared" si="11"/>
@@ -11201,7 +11201,7 @@
       </c>
       <c r="G59">
         <f t="shared" si="12"/>
-        <v>0.4560311482768164</v>
+        <v>1.0563354922519788</v>
       </c>
       <c r="H59">
         <f t="shared" si="12"/>
@@ -11250,7 +11250,7 @@
       </c>
       <c r="G60">
         <f t="shared" si="12"/>
-        <v>0.45496375515726656</v>
+        <v>1.0538630180786102</v>
       </c>
       <c r="H60">
         <f t="shared" si="12"/>
@@ -11299,7 +11299,7 @@
       </c>
       <c r="G61">
         <f t="shared" si="12"/>
-        <v>0.4538883331707374</v>
+        <v>1.0513719461029098</v>
       </c>
       <c r="H61">
         <f t="shared" si="12"/>
@@ -11348,7 +11348,7 @@
       </c>
       <c r="G62">
         <f t="shared" si="12"/>
-        <v>0.45280579021800071</v>
+        <v>1.0488643793562435</v>
       </c>
       <c r="H62">
         <f t="shared" si="12"/>
@@ -11397,7 +11397,7 @@
       </c>
       <c r="G63">
         <f t="shared" si="13"/>
-        <v>0.45171693153480535</v>
+        <v>1.0463421830601083</v>
       </c>
       <c r="H63">
         <f t="shared" si="13"/>
@@ -11446,7 +11446,7 @@
       </c>
       <c r="G64">
         <f t="shared" si="13"/>
-        <v>0.45062247130119337</v>
+        <v>1.0438070115175695</v>
       </c>
       <c r="H64">
         <f t="shared" si="13"/>
@@ -11495,7 +11495,7 @@
       </c>
       <c r="G65">
         <f t="shared" si="13"/>
-        <v>0.44952304293803963</v>
+        <v>1.0412603319638236</v>
       </c>
       <c r="H65">
         <f t="shared" si="13"/>
@@ -11544,7 +11544,7 @@
       </c>
       <c r="G66">
         <f t="shared" si="13"/>
-        <v>0.44841920823926296</v>
+        <v>1.0387034457197521</v>
       </c>
       <c r="H66">
         <f t="shared" si="13"/>
@@ -11593,7 +11593,7 @@
       </c>
       <c r="G67">
         <f t="shared" si="14"/>
-        <v>0.44731146547137141</v>
+        <v>1.0361375069534402</v>
       </c>
       <c r="H67">
         <f t="shared" si="14"/>
@@ -11642,7 +11642,7 @@
       </c>
       <c r="G68">
         <f t="shared" si="14"/>
-        <v>0.44620025655711376</v>
+        <v>1.033563539320149</v>
       </c>
       <c r="H68">
         <f t="shared" si="14"/>
@@ -11691,7 +11691,7 @@
       </c>
       <c r="G69">
         <f t="shared" si="14"/>
-        <v>0.44508597344680723</v>
+        <v>1.03098245072065</v>
       </c>
       <c r="H69">
         <f t="shared" si="14"/>
@@ -11740,7 +11740,7 @@
       </c>
       <c r="G70">
         <f t="shared" si="14"/>
-        <v>0.44396896376919859</v>
+        <v>1.0283950463906926</v>
       </c>
       <c r="H70">
         <f t="shared" si="14"/>
@@ -11789,7 +11789,7 @@
       </c>
       <c r="G71">
         <f t="shared" si="16"/>
-        <v>0.44284953584332748</v>
+        <v>1.0258020405103181</v>
       </c>
       <c r="H71">
         <f t="shared" si="16"/>
@@ -11838,7 +11838,7 @@
       </c>
       <c r="G72">
         <f t="shared" si="16"/>
-        <v>0.44172796312365159</v>
+        <v>1.0232040665004023</v>
       </c>
       <c r="H72">
         <f t="shared" si="16"/>
@@ -11887,7 +11887,7 @@
       </c>
       <c r="G73">
         <f t="shared" si="16"/>
-        <v>0.44060448814251746</v>
+        <v>1.0206016861548635</v>
       </c>
       <c r="H73">
         <f t="shared" si="16"/>
@@ -11936,7 +11936,7 @@
       </c>
       <c r="G74">
         <f t="shared" si="16"/>
-        <v>0.43947932600682005</v>
+        <v>1.0179953977402094</v>
       </c>
       <c r="H74">
         <f t="shared" si="16"/>
@@ -11985,7 +11985,7 @@
       </c>
       <c r="G75">
         <f t="shared" si="17"/>
-        <v>0.43835266749926072</v>
+        <v>1.0153856431791897</v>
       </c>
       <c r="H75">
         <f t="shared" si="17"/>
@@ -12034,7 +12034,7 @@
       </c>
       <c r="G76">
         <f t="shared" si="17"/>
-        <v>0.43722468182891611</v>
+        <v>1.0127728144221211</v>
       </c>
       <c r="H76">
         <f t="shared" si="17"/>
@@ -12083,7 +12083,7 @@
       </c>
       <c r="G77">
         <f t="shared" si="17"/>
-        <v>0.43609551907077426</v>
+        <v>1.0101572590977501</v>
       </c>
       <c r="H77">
         <f t="shared" si="17"/>
@@ -12132,7 +12132,7 @@
       </c>
       <c r="G78">
         <f t="shared" si="17"/>
-        <v>0.43496531232940927</v>
+        <v>1.0075392855251168</v>
       </c>
       <c r="H78">
         <f t="shared" si="17"/>
@@ -12181,7 +12181,7 @@
       </c>
       <c r="G79">
         <f t="shared" si="18"/>
-        <v>0.43383417965798798</v>
+        <v>1.0049191671586786</v>
       </c>
       <c r="H79">
         <f t="shared" si="18"/>
@@ -12230,7 +12230,7 @@
       </c>
       <c r="G80">
         <f t="shared" si="18"/>
-        <v>0.432702225760277</v>
+        <v>1.0022971465307822</v>
       </c>
       <c r="H80">
         <f t="shared" si="18"/>
@@ -12279,7 +12279,7 @@
       </c>
       <c r="G81">
         <f t="shared" si="18"/>
-        <v>0.43156954350018645</v>
+        <v>0.99967343874832271</v>
       </c>
       <c r="H81">
         <f t="shared" si="18"/>
@@ -12328,7 +12328,7 @@
       </c>
       <c r="G82">
         <f t="shared" si="18"/>
-        <v>0.43043621524061609</v>
+        <v>0.99704823459400105</v>
       </c>
       <c r="H82">
         <f t="shared" si="18"/>
@@ -12377,7 +12377,7 @@
       </c>
       <c r="G83">
         <f t="shared" si="19"/>
-        <v>0.42930231403090502</v>
+        <v>0.99442170327689428</v>
       </c>
       <c r="H83">
         <f t="shared" si="19"/>
@@ -12426,7 +12426,7 @@
       </c>
       <c r="G84">
         <f t="shared" si="19"/>
-        <v>0.42816790466000493</v>
+        <v>0.99179399487199016</v>
       </c>
       <c r="H84">
         <f t="shared" si="19"/>
@@ -12475,7 +12475,7 @@
       </c>
       <c r="G85">
         <f t="shared" si="19"/>
-        <v>0.42703304459056107</v>
+        <v>0.98916524248386295</v>
       </c>
       <c r="H85">
         <f t="shared" si="19"/>
@@ -12524,7 +12524,7 @@
       </c>
       <c r="G86">
         <f t="shared" si="19"/>
-        <v>0.42589778478736806</v>
+        <v>0.98653556416567967</v>
       </c>
       <c r="H86">
         <f t="shared" si="19"/>
@@ -12573,7 +12573,7 @@
       </c>
       <c r="G87">
         <f t="shared" si="20"/>
-        <v>0.42476217045214348</v>
+        <v>0.98390506462120619</v>
       </c>
       <c r="H87">
         <f t="shared" si="20"/>
@@ -12622,7 +12622,7 @@
       </c>
       <c r="G88">
         <f t="shared" si="20"/>
-        <v>0.42362624167521495</v>
+        <v>0.98127383671435364</v>
       </c>
       <c r="H88">
         <f t="shared" si="20"/>
@@ -12671,7 +12671,7 @@
       </c>
       <c r="G89">
         <f t="shared" si="20"/>
-        <v>0.42249003401351271</v>
+        <v>0.97864196280802096</v>
       </c>
       <c r="H89">
         <f t="shared" si="20"/>
@@ -12720,7 +12720,7 @@
       </c>
       <c r="G90">
         <f t="shared" si="20"/>
-        <v>0.42135357900320541</v>
+        <v>0.97600951595154772</v>
       </c>
       <c r="H90">
         <f t="shared" si="20"/>
@@ -12769,7 +12769,7 @@
       </c>
       <c r="G91">
         <f t="shared" si="21"/>
-        <v>0.42021690461436517</v>
+        <v>0.97337656093388536</v>
       </c>
       <c r="H91">
         <f t="shared" si="21"/>
@@ -12818,7 +12818,7 @@
       </c>
       <c r="G92">
         <f t="shared" si="21"/>
-        <v>0.4190800356542207</v>
+        <v>0.97074315521767929</v>
       </c>
       <c r="H92">
         <f t="shared" si="21"/>
@@ -12867,7 +12867,7 @@
       </c>
       <c r="G93">
         <f t="shared" si="21"/>
-        <v>0.41794299412481017</v>
+        <v>0.96810934976772411</v>
       </c>
       <c r="H93">
         <f t="shared" si="21"/>
@@ -12916,7 +12916,7 @@
       </c>
       <c r="G94">
         <f t="shared" si="21"/>
-        <v>0.4168057995401907</v>
+        <v>0.9654751897857371</v>
       </c>
       <c r="H94">
         <f t="shared" si="21"/>
@@ -12965,7 +12965,7 @@
       </c>
       <c r="G95">
         <f t="shared" si="22"/>
-        <v>0.41566846920777861</v>
+        <v>0.96284071536204641</v>
       </c>
       <c r="H95">
         <f t="shared" si="22"/>
@@ -13014,7 +13014,7 @@
       </c>
       <c r="G96">
         <f t="shared" si="22"/>
-        <v>0.41453101847787499</v>
+        <v>0.960205962053582</v>
       </c>
       <c r="H96">
         <f t="shared" si="22"/>
@@ -13063,7 +13063,7 @@
       </c>
       <c r="G97">
         <f t="shared" si="22"/>
-        <v>0.41339346096497559</v>
+        <v>0.95757096139651265</v>
       </c>
       <c r="H97">
         <f t="shared" si="22"/>
@@ -13112,7 +13112,7 @@
       </c>
       <c r="G98">
         <f t="shared" si="22"/>
-        <v>0.41225580874405476</v>
+        <v>0.95493574136090997</v>
       </c>
       <c r="H98">
         <f t="shared" si="22"/>
@@ -13161,7 +13161,7 @@
       </c>
       <c r="G99">
         <f t="shared" si="23"/>
-        <v>0.41111807252465449</v>
+        <v>0.95230032675400345</v>
       </c>
       <c r="H99">
         <f t="shared" si="23"/>
@@ -13210,7 +13210,7 @@
       </c>
       <c r="G100">
         <f t="shared" si="23"/>
-        <v>0.40998026180528591</v>
+        <v>0.94966473957783049</v>
       </c>
       <c r="H100">
         <f t="shared" si="23"/>
@@ -13259,7 +13259,7 @@
       </c>
       <c r="G101">
         <f t="shared" si="23"/>
-        <v>0.40884238501037318</v>
+        <v>0.94702899934644913</v>
       </c>
       <c r="H101">
         <f t="shared" si="23"/>
@@ -13308,7 +13308,7 @@
       </c>
       <c r="G102">
         <f t="shared" si="23"/>
-        <v>0.40770444961170965</v>
+        <v>0.94439312336727477</v>
       </c>
       <c r="H102">
         <f t="shared" si="23"/>
@@ -13357,7 +13357,7 @@
       </c>
       <c r="G103">
         <f t="shared" si="24"/>
-        <v>0.40656646223618209</v>
+        <v>0.94175712699060887</v>
       </c>
       <c r="H103">
         <f t="shared" si="24"/>

</xml_diff>